<commit_message>
Updated the excel template to v6
</commit_message>
<xml_diff>
--- a/assets/files/sawaliram_template.xlsx
+++ b/assets/files/sawaliram_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21323"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BCEF3F7-8445-4DAB-B9B0-50B24DD8EE88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Question Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -87,8 +86,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,17 +102,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,10 +138,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,41 +464,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4847EE86-B175-45CB-A771-E136A969C9C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0" xr3:uid="{758FD503-BFA7-50B8-9ED7-D53CECBD4920}">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="7" max="9" width="27.28515625" customWidth="1"/>
-    <col min="10" max="11" width="32" customWidth="1"/>
-    <col min="12" max="12" width="27.42578125" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" customWidth="1"/>
-    <col min="16" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="47.7109375" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" customWidth="1"/>
-    <col min="20" max="20" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="54" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28" style="5" customWidth="1"/>
+    <col min="7" max="9" width="27.33203125" style="4" customWidth="1"/>
+    <col min="10" max="11" width="32" style="4" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="47.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="27.109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="28.44140625" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +517,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -518,7 +550,7 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -531,56 +563,62 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="F2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R2" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="27">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The question asked, in its original language" sqref="A1:A1048576" xr:uid="{26C97BEE-7063-48E6-905D-F196831377CF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Original language of the question" sqref="B1:B1048576" xr:uid="{F4D3518E-C733-4E05-8E99-CC4AB86C6548}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Translation of the question in English. Leave blank if the original question is in English." sqref="C1:C1048576" xr:uid="{FD6ACC32-51C7-4AC1-BE68-03B6EE52BBCE}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Format in which the question was asked. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="D2:D1048576" xr:uid="{B70ED986-9957-4E79-AE63-19FDE4EE328F}">
+  <sheetProtection selectLockedCells="1"/>
+  <dataValidations count="29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Format in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="D2:D5 D7:D1048576">
+      <formula1>"Handed over in written form, Asked orally, Received by post"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The setting in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of publication (dd/mm/yyyy). Leave blank if not published." sqref="Q1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date on which the question was asked, in the format dd-mm-yyyy" sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The curriculum of the school. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="K1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The setting in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="E2:E6 E7:E1048576">
+      <formula1>"In class, During or after an activity or field trip, During or after a special event, Other (elaborate in the Notes column)"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Format in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="D6">
       <formula1>"Handed over in written form,Asked orally,Received by post"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Format in which the question was asked. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="D1" xr:uid="{927D8E90-0C82-41F6-BFF8-A5625F0469D5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The setting in which the question was asked. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="E1" xr:uid="{401B2E37-9543-4578-8C14-31B8C4FCA0A7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O1" xr:uid="{136DC51C-1501-42CE-BBAC-51DEB08980DB}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O2:O1048576" xr:uid="{CE1A9351-362B-4432-9B4D-8DD40C661B2F}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The question as asked, in its original language" sqref="A1:A1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Original language of the question" sqref="B1:B1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Translation of the question in English. Leave blank if the original question is in English." sqref="C1:C1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Leave blank if not published." sqref="P1:P1048576" xr:uid="{558E9E1A-BBB0-40C3-B317-54B8FBEE0FC6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of publication (dd/mm/yyyy). Leave blank if not published." sqref="Q1" xr:uid="{8AF1D1B1-D92F-498A-AAC9-C5AE83F3516B}"/>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published." sqref="Q2:Q1048576" xr:uid="{CBADB448-0DE5-4497-9FD7-C69032EB59A4}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Leave blank if not published." sqref="P1:P1048576"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published." sqref="Q2:Q3 Q5:Q1048576">
       <formula1>1</formula1>
       <formula2>109939</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date on which the question was asked, in the format dd-mm-yyyy" sqref="F1" xr:uid="{475D77AD-B7DB-4CC1-AB2E-484E0E7EE3D1}"/>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date on which the question was asked, in the format dd-mm-yyyy" sqref="F2:F1048576" xr:uid="{284C800C-58F6-4F59-A907-732CDE7213D7}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="The date on which the question was asked, in the format dd-mm-yyyy" sqref="F2:F1048576">
       <formula1>1</formula1>
       <formula2>109939</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of the student(s) who asked the question (may be entered in the local language). If multiple students have asked the same question, enter their names as a comma-separated list, eg: Geeta, Ali, Mary." sqref="G1:G1048576" xr:uid="{35EBAAF7-689E-4BD4-A26E-F6F565AB8EE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question. If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation, Eg: 7, 8, 9, 10." sqref="I1:I1048576" xr:uid="{85835FF5-0B6D-4E08-9AF0-D15AFB9DD76E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the school the student is enrolled in (may be entered in the local language)." sqref="J1:J1048576" xr:uid="{96A2C8BB-2D4A-451D-ABD8-50F48913D193}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school" sqref="L1:L1048576" xr:uid="{C53E6673-0EAF-40F3-AA99-5B3A5FCF94D4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The address of the student’s school or residence (locality/village-town-city/district). May be entered in local language." sqref="M1:M1048576" xr:uid="{DFC09F77-4AE3-4222-9F95-69BA765AA858}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located. May be entered in local language." sqref="N1:N1048576" xr:uid="{884512EE-EB4E-4B0E-ABD6-742566B93726}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the person who collected/received the question." sqref="S1:S1048576" xr:uid="{7FFD3CE2-4D62-4B1D-A277-143A118B3567}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The curriculum of the school. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="K2:K1048576" xr:uid="{D51E207D-4C30-4198-AE69-9E9F00D5F981}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of the student(s) who asked the question (may be entered in the local language). If multiple students have asked the same question, enter their names as a comma-separated list, eg: Geeta, Ali, Mary." sqref="G1:G1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question. If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation, Eg: 7, 8, 9, 10." sqref="I1:I1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the school the student is enrolled in (may be entered in the local language)." sqref="J1:J1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school" sqref="L1:L1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The address of the student’s school or residence (locality/village-town-city/district). May be entered in local language." sqref="M1:M1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located. May be entered in local language." sqref="N1:N1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Name of the person who collected/entered the question." sqref="S1:S1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The curriculum of the school. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="K2:K1048576">
       <formula1>"State Board, CBSE, ICSE, HSTP, Small Science, Other (elaborate in the Notes column)"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The curriculum of the school. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="K1" xr:uid="{98995C10-72DF-401D-A5A6-D25BB409CF65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Space for additional details or information points not recorded in any other field. Use semicolon (;) as a separator for more than one point." sqref="R1:R1048576" xr:uid="{F4A307E1-9F3D-489B-93B0-9459E11C40DE}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The setting in which the question was asked. Choose one of the options listed. (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="E2:E1048576" xr:uid="{0E1F5075-EF7C-4581-A29F-F7EBEC986761}">
-      <formula1>"In class, During or after an activity or field trip, During or after a special event, Other (elaborate in the Notes column)"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of the student who asked the question (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="H1" xr:uid="{F1A1940D-AE52-4022-851F-ABF60345702A}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Gender of the student who asked the question (Click on the drop-down menu to the right of the cell or press Alt + Down Arrow)" sqref="H2:H1048576" xr:uid="{B4928DF9-CB23-4AD5-B170-245A198C7D3A}">
-      <formula1>"Male,Female"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Role of the person who received/collected the question, eg: teacher, volunteer, AFSP, project officer, etc." sqref="T1:T1048576" xr:uid="{FD5E35F6-ACA1-4017-BBA1-2974A78B55DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Space for additional details or information points not recorded in any other field. Use semicolon (;) as a separator for more than one point." sqref="R1:R1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H2:H1048576">
+      <formula1>"Male, Female"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question, eg: teacher, volunteer, AFSP, project officer, etc." sqref="T1:T1048576"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published" sqref="Q4">
+      <formula1>1</formula1>
+      <formula2>109939</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revised template and guidelines_Jan 2021
The help text and drop-down options of some fields have been revised. Along with the updated guidelines with a checklist for the 20 fields.
</commit_message>
<xml_diff>
--- a/assets/files/sawaliram_template.xlsx
+++ b/assets/files/sawaliram_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_TIFRH\Sawaliram\Databases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Question Data" sheetId="2" r:id="rId1"/>
@@ -31,9 +26,6 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Question Language</t>
-  </si>
-  <si>
     <t>English translation of the question</t>
   </si>
   <si>
@@ -46,18 +38,9 @@
     <t>Date of asking the question</t>
   </si>
   <si>
-    <t>Student Name</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Student Class</t>
-  </si>
-  <si>
-    <t>School Name</t>
-  </si>
-  <si>
     <t>Curriculum followed</t>
   </si>
   <si>
@@ -73,19 +56,31 @@
     <t>Published (Yes/No)</t>
   </si>
   <si>
-    <t>Publication Name</t>
-  </si>
-  <si>
-    <t>Publication Date</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Contributor Name</t>
-  </si>
-  <si>
-    <t>Contributor Role</t>
+    <t>Student class</t>
+  </si>
+  <si>
+    <t>Question language</t>
+  </si>
+  <si>
+    <t>Student name</t>
+  </si>
+  <si>
+    <t>School name</t>
+  </si>
+  <si>
+    <t>Publication name</t>
+  </si>
+  <si>
+    <t>Publication date</t>
+  </si>
+  <si>
+    <t>Contributor name</t>
+  </si>
+  <si>
+    <t>Contributor role</t>
   </si>
 </sst>
 </file>
@@ -469,7 +464,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -481,85 +476,85 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="54" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="4" customWidth="1"/>
     <col min="6" max="6" width="28" style="5" customWidth="1"/>
-    <col min="7" max="9" width="27.28515625" style="4" customWidth="1"/>
+    <col min="7" max="9" width="27.33203125" style="4" customWidth="1"/>
     <col min="10" max="11" width="32" style="4" customWidth="1"/>
-    <col min="12" max="12" width="27.42578125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="47.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="28.42578125" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="4"/>
+    <col min="12" max="12" width="27.44140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="47.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="27.109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="28.44140625" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>18</v>
@@ -568,12 +563,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
       <c r="R2" s="6"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <dataValidations count="29">
+  <dataValidations xWindow="1757" yWindow="336" count="30">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Format in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="D2:D5 D7:D1048576">
       <formula1>"Handed over in written form, Asked orally, Received by post"</formula1>
     </dataValidation>
@@ -596,7 +591,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Leave blank if not published." sqref="P1:P1048576"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published." sqref="Q2:Q3 Q5:Q1048576">
       <formula1>1</formula1>
       <formula2>109939</formula2>
@@ -606,24 +600,28 @@
       <formula2>109939</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of the student(s) who asked the question (may be entered in the local language). If multiple students have asked the same question, enter their names as a comma-separated list, eg: Geeta, Ali, Mary." sqref="G1:G1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question. If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation, Eg: 7, 8, 9, 10." sqref="I1:I1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the school the student is enrolled in (may be entered in the local language)." sqref="J1:J1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school" sqref="L1:L1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school (enter the language in Roman script)._x000a_" sqref="L1:L1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The address of the student’s school or residence (locality/village-town-city/district). May be entered in local language." sqref="M1:M1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located. May be entered in local language." sqref="N1:N1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located, in English. " sqref="N1:N1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Name of the person who collected/entered the question." sqref="S1:S1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The curriculum of the school. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="K2:K1048576">
-      <formula1>"State Board, CBSE, ICSE, HSTP, Small Science, Other (elaborate in the Notes column)"</formula1>
+      <formula1>"State Board, CBSE, ICSE, HSTP, Small Science, IGCSE, Edexcel, Other (Specify the curriculum in the Notes column) "</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Space for additional details or information points not recorded in any other field. Use semicolon (;) as a separator for more than one point." sqref="R1:R1048576"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H2:H1048576">
-      <formula1>"Male, Female"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question, eg: teacher, volunteer, AFSP, project officer, etc." sqref="T1:T1048576"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published" sqref="Q4">
       <formula1>1</formula1>
       <formula2>109939</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H2:H1048576">
+      <formula1>"Male, Female, Non-binary"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question. " sqref="T2:T1048576">
+      <formula1>"Teacher, Principal / Mentor, Project staff, Volunteer, Expert, Researcher, Parent "</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question. " sqref="T1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Include details of issue or volume separated by a semicolon. Leave blank if not published." sqref="P1:P1048576 P1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question (Nursery, Preschool, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12). If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation. " sqref="I1:I1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reverting last 4 commits
</commit_message>
<xml_diff>
--- a/assets/files/sawaliram_template.xlsx
+++ b/assets/files/sawaliram_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_TIFRH\Sawaliram\Databases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Question Data" sheetId="2" r:id="rId1"/>
@@ -26,6 +31,9 @@
     <t>Question</t>
   </si>
   <si>
+    <t>Question Language</t>
+  </si>
+  <si>
     <t>English translation of the question</t>
   </si>
   <si>
@@ -38,9 +46,18 @@
     <t>Date of asking the question</t>
   </si>
   <si>
+    <t>Student Name</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
+    <t>Student Class</t>
+  </si>
+  <si>
+    <t>School Name</t>
+  </si>
+  <si>
     <t>Curriculum followed</t>
   </si>
   <si>
@@ -56,31 +73,19 @@
     <t>Published (Yes/No)</t>
   </si>
   <si>
+    <t>Publication Name</t>
+  </si>
+  <si>
+    <t>Publication Date</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Student class</t>
-  </si>
-  <si>
-    <t>Question language</t>
-  </si>
-  <si>
-    <t>Student name</t>
-  </si>
-  <si>
-    <t>School name</t>
-  </si>
-  <si>
-    <t>Publication name</t>
-  </si>
-  <si>
-    <t>Publication date</t>
-  </si>
-  <si>
-    <t>Contributor name</t>
-  </si>
-  <si>
-    <t>Contributor role</t>
+    <t>Contributor Name</t>
+  </si>
+  <si>
+    <t>Contributor Role</t>
   </si>
 </sst>
 </file>
@@ -464,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,85 +481,85 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.88671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="63.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="54" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="28" style="5" customWidth="1"/>
-    <col min="7" max="9" width="27.33203125" style="4" customWidth="1"/>
+    <col min="7" max="9" width="27.28515625" style="4" customWidth="1"/>
     <col min="10" max="11" width="32" style="4" customWidth="1"/>
-    <col min="12" max="12" width="27.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="29.44140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="27.33203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="18.109375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="47.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="27.109375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="28.44140625" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="27.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="47.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="28.42578125" style="4" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>18</v>
@@ -563,12 +568,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="13.9" x14ac:dyDescent="0.25">
       <c r="R2" s="6"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <dataValidations xWindow="1757" yWindow="336" count="30">
+  <dataValidations count="29">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click on the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Format in which the question was asked. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="D2:D5 D7:D1048576">
       <formula1>"Handed over in written form, Asked orally, Received by post"</formula1>
     </dataValidation>
@@ -591,6 +596,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Has the question been published in a magazine, book, newspaper or website? Select Yes/No." sqref="O2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Leave blank if not published." sqref="P1:P1048576"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published." sqref="Q2:Q3 Q5:Q1048576">
       <formula1>1</formula1>
       <formula2>109939</formula2>
@@ -600,28 +606,24 @@
       <formula2>109939</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of the student(s) who asked the question (may be entered in the local language). If multiple students have asked the same question, enter their names as a comma-separated list, eg: Geeta, Ali, Mary." sqref="G1:G1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question. If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation, Eg: 7, 8, 9, 10." sqref="I1:I1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the school the student is enrolled in (may be entered in the local language)." sqref="J1:J1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school (enter the language in Roman script)._x000a_" sqref="L1:L1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Language in which classes are taught in the school" sqref="L1:L1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The address of the student’s school or residence (locality/village-town-city/district). May be entered in local language." sqref="M1:M1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located, in English. " sqref="N1:N1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The state in India where the school/residence is located. May be entered in local language." sqref="N1:N1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Name of the person who collected/entered the question." sqref="S1:S1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="The curriculum of the school. Choose one of the options listed. (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="K2:K1048576">
-      <formula1>"State Board, CBSE, ICSE, HSTP, Small Science, IGCSE, Edexcel, Other (Specify the curriculum in the Notes column) "</formula1>
+      <formula1>"State Board, CBSE, ICSE, HSTP, Small Science, Other (elaborate in the Notes column)"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Space for additional details or information points not recorded in any other field. Use semicolon (;) as a separator for more than one point." sqref="R1:R1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field has drop-down options" error="Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H2:H1048576">
+      <formula1>"Male, Female"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question, eg: teacher, volunteer, AFSP, project officer, etc." sqref="T1:T1048576"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Accepted format is dd-mm-yyyy" prompt="Date of publication (dd-mm-yyyy). Leave blank if not published" sqref="Q4">
       <formula1>1</formula1>
       <formula2>109939</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Gender of the student who asked the question (Click the drop-down menu to the right of the cell or press 'Alt+Down arrow' for options)" sqref="H2:H1048576">
-      <formula1>"Male, Female, Non-binary"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question. " sqref="T2:T1048576">
-      <formula1>"Teacher, Principal / Mentor, Project staff, Volunteer, Expert, Researcher, Parent "</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="Role of the person who collected/entered the question. " sqref="T1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the publication in which the question appeared. Include details of issue or volume separated by a semicolon. Leave blank if not published." sqref="P1:P1048576 P1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class of the student(s) who asked the question (Nursery, Preschool, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12). If the class of that student is not known but the group had students from multiple classes, enter the classes with comma-separation. " sqref="I1:I1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>